<commit_message>
masterFile uploaded for weekly processes
</commit_message>
<xml_diff>
--- a/MichiganVsMSUFile.xlsx
+++ b/MichiganVsMSUFile.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lissjust/Documents/NCAAWomens/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA6C9EE3-8FAE-ED43-B547-687F765A930B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5127374-7DDF-7D44-AE61-F9E7D57B1E32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{91DD581D-37E4-6C49-9749-B261A19E9776}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{91DD581D-37E4-6C49-9749-B261A19E9776}"/>
   </bookViews>
   <sheets>
     <sheet name="Michigan @ MSU" sheetId="3" r:id="rId1"/>
     <sheet name="Rotations" sheetId="4" r:id="rId2"/>
-    <sheet name="Player Rotations" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -3376,8 +3375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9A378DC-DBA7-8749-80FC-836ED6ECB66A}">
   <dimension ref="B7:BV103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="I86" sqref="I86"/>
+    <sheetView topLeftCell="A10" zoomScale="163" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9902,8 +9901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D157CF-02E9-9D41-9BC8-64993BCF9970}">
   <dimension ref="B11:AR76"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="L113" sqref="L113"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10125,320 +10124,320 @@
     </row>
     <row r="14" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B14" s="191" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C14" s="192" t="str">
         <f>VLOOKUP($B14,$B$63:$AA$76,C$11,FALSE)</f>
-        <v>G</v>
+        <v>F</v>
       </c>
       <c r="D14" s="192" t="str">
         <f>VLOOKUP($B14,$B$63:$AA$76,D$11,FALSE)</f>
-        <v>6'0"</v>
+        <v>6'2"</v>
       </c>
       <c r="E14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,E$11,FALSE)</f>
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="F14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,F$11,FALSE)</f>
-        <v>5.2</v>
+        <v>22.9</v>
       </c>
       <c r="G14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,G$11,FALSE)</f>
-        <v>0.5</v>
+        <v>5.4</v>
       </c>
       <c r="H14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,H$11,FALSE)</f>
-        <v>1.9</v>
+        <v>8.6</v>
       </c>
       <c r="I14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,I$11,FALSE)</f>
-        <v>25.8</v>
+        <v>62.8</v>
       </c>
       <c r="J14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,J$11,FALSE)</f>
-        <v>0.2</v>
+        <v>5.4</v>
       </c>
       <c r="K14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,K$11,FALSE)</f>
-        <v>0.6</v>
+        <v>8.6</v>
       </c>
       <c r="L14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,L$11,FALSE)</f>
-        <v>40</v>
+        <v>62.8</v>
       </c>
       <c r="M14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,M$11,FALSE)</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="N14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,N$11,FALSE)</f>
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="O14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,O$11,FALSE)</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="P14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,P$11,FALSE)</f>
-        <v>0.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="Q14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,Q$11,FALSE)</f>
-        <v>0.2</v>
+        <v>3.7</v>
       </c>
       <c r="R14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,R$11,FALSE)</f>
-        <v>25</v>
+        <v>63.2</v>
       </c>
       <c r="S14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,S$11,FALSE)</f>
-        <v>0.3</v>
+        <v>3.6</v>
       </c>
       <c r="T14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,T$11,FALSE)</f>
-        <v>0.2</v>
+        <v>3.4</v>
       </c>
       <c r="U14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,U$11,FALSE)</f>
-        <v>0.6</v>
+        <v>7</v>
       </c>
       <c r="V14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,V$11,FALSE)</f>
-        <v>0.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="W14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,W$11,FALSE)</f>
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="X14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,X$11,FALSE)</f>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="Y14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,Y$11,FALSE)</f>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="Z14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,Z$11,FALSE)</f>
-        <v>0.2</v>
+        <v>2.4</v>
       </c>
       <c r="AA14" s="192">
         <f>VLOOKUP($B14,$B$63:$AA$76,AA$11,FALSE)</f>
-        <v>1.3</v>
+        <v>13.1</v>
       </c>
       <c r="AC14">
         <f t="shared" ref="AC14:AC18" si="0">$S14/$F14</f>
-        <v>5.7692307692307689E-2</v>
+        <v>0.15720524017467249</v>
       </c>
       <c r="AD14">
         <f t="shared" ref="AD14:AD18" si="1">$T14/$F14</f>
-        <v>3.8461538461538464E-2</v>
+        <v>0.14847161572052403</v>
       </c>
       <c r="AE14">
         <f t="shared" ref="AE14:AE18" si="2">$G14/$F14</f>
-        <v>9.6153846153846145E-2</v>
+        <v>0.23580786026200876</v>
       </c>
       <c r="AF14">
         <f t="shared" ref="AF14:AF18" si="3">$H14/$F14</f>
-        <v>0.36538461538461536</v>
+        <v>0.37554585152838427</v>
       </c>
       <c r="AG14">
         <f t="shared" ref="AG14:AG18" si="4">$J14/$F14</f>
-        <v>3.8461538461538464E-2</v>
+        <v>0.23580786026200876</v>
       </c>
       <c r="AH14">
         <f t="shared" ref="AH14:AH18" si="5">$K14/$F14</f>
-        <v>0.11538461538461538</v>
+        <v>0.37554585152838427</v>
       </c>
       <c r="AI14">
         <f t="shared" ref="AI14:AI18" si="6">$M14/$F14</f>
-        <v>3.8461538461538464E-2</v>
+        <v>0</v>
       </c>
       <c r="AJ14">
         <f t="shared" ref="AJ14:AJ18" si="7">$N14/$F14</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AK14">
         <f t="shared" ref="AK14:AK18" si="8">$P14/$F14</f>
-        <v>1.9230769230769232E-2</v>
+        <v>0.10043668122270742</v>
       </c>
       <c r="AL14">
         <f t="shared" ref="AL14:AL18" si="9">$Q14/$F14</f>
-        <v>3.8461538461538464E-2</v>
+        <v>0.16157205240174674</v>
       </c>
       <c r="AM14">
         <f t="shared" ref="AM14:AM18" si="10">$V14/$F14</f>
-        <v>7.6923076923076927E-2</v>
+        <v>4.8034934497816602E-2</v>
       </c>
       <c r="AN14">
         <f t="shared" ref="AN14:AN17" si="11">$W15/$F15</f>
-        <v>6.5217391304347824E-2</v>
+        <v>8.3650190114068448E-2</v>
       </c>
       <c r="AO14">
         <f t="shared" ref="AO14:AO18" si="12">$X14/$F14</f>
-        <v>1.9230769230769232E-2</v>
+        <v>4.3668122270742363E-2</v>
       </c>
       <c r="AP14">
         <f>Y14/F14</f>
-        <v>1.9230769230769232E-2</v>
+        <v>8.7336244541484729E-3</v>
       </c>
       <c r="AQ14">
         <f t="shared" ref="AQ14:AQ18" si="13">Z14/F14</f>
-        <v>3.8461538461538464E-2</v>
+        <v>0.10480349344978167</v>
       </c>
       <c r="AR14">
         <f t="shared" ref="AR14:AR18" si="14">AA14/F14</f>
-        <v>0.25</v>
+        <v>0.57205240174672489</v>
       </c>
     </row>
     <row r="15" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B15" s="191" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C15" s="192" t="str">
         <f>VLOOKUP($B15,$B$63:$AA$76,C$11,FALSE)</f>
-        <v>F</v>
+        <v>G</v>
       </c>
       <c r="D15" s="192" t="str">
         <f>VLOOKUP($B15,$B$63:$AA$76,D$11,FALSE)</f>
-        <v>6'3"</v>
+        <v>5'10"</v>
       </c>
       <c r="E15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,E$11,FALSE)</f>
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="F15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,F$11,FALSE)</f>
-        <v>4.5999999999999996</v>
+        <v>26.3</v>
       </c>
       <c r="G15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,G$11,FALSE)</f>
-        <v>0.6</v>
+        <v>3</v>
       </c>
       <c r="H15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,H$11,FALSE)</f>
-        <v>1.4</v>
+        <v>7.9</v>
       </c>
       <c r="I15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,I$11,FALSE)</f>
-        <v>44</v>
+        <v>38.1</v>
       </c>
       <c r="J15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,J$11,FALSE)</f>
-        <v>0.6</v>
+        <v>2.4</v>
       </c>
       <c r="K15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,K$11,FALSE)</f>
-        <v>1.4</v>
+        <v>5.9</v>
       </c>
       <c r="L15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,L$11,FALSE)</f>
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="M15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,M$11,FALSE)</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="N15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,N$11,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,O$11,FALSE)</f>
-        <v>0</v>
+        <v>32.4</v>
       </c>
       <c r="P15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,P$11,FALSE)</f>
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,Q$11,FALSE)</f>
-        <v>0.9</v>
+        <v>2.6</v>
       </c>
       <c r="R15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,R$11,FALSE)</f>
-        <v>70.599999999999994</v>
+        <v>75.3</v>
       </c>
       <c r="S15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,S$11,FALSE)</f>
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="T15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,T$11,FALSE)</f>
-        <v>0.7</v>
+        <v>3.2</v>
       </c>
       <c r="U15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,U$11,FALSE)</f>
-        <v>1.6</v>
+        <v>3.9</v>
       </c>
       <c r="V15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,V$11,FALSE)</f>
-        <v>0.3</v>
+        <v>2.4</v>
       </c>
       <c r="W15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,W$11,FALSE)</f>
-        <v>0.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="X15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,X$11,FALSE)</f>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="Y15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,Y$11,FALSE)</f>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="Z15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,Z$11,FALSE)</f>
-        <v>0.3</v>
+        <v>2.6</v>
       </c>
       <c r="AA15" s="192">
         <f>VLOOKUP($B15,$B$63:$AA$76,AA$11,FALSE)</f>
-        <v>1.9</v>
+        <v>8.6</v>
       </c>
       <c r="AC15">
         <f t="shared" si="0"/>
-        <v>0.19565217391304349</v>
+        <v>2.6615969581749048E-2</v>
       </c>
       <c r="AD15">
         <f t="shared" si="1"/>
-        <v>0.15217391304347827</v>
+        <v>0.12167300380228137</v>
       </c>
       <c r="AE15">
         <f t="shared" si="2"/>
-        <v>0.13043478260869565</v>
+        <v>0.11406844106463879</v>
       </c>
       <c r="AF15">
         <f t="shared" si="3"/>
-        <v>0.30434782608695654</v>
+        <v>0.30038022813688214</v>
       </c>
       <c r="AG15">
         <f t="shared" si="4"/>
-        <v>0.13043478260869565</v>
+        <v>9.1254752851711016E-2</v>
       </c>
       <c r="AH15">
         <f t="shared" si="5"/>
-        <v>0.30434782608695654</v>
+        <v>0.22433460076045628</v>
       </c>
       <c r="AI15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.2813688212927754E-2</v>
       </c>
       <c r="AJ15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>7.6045627376425853E-2</v>
       </c>
       <c r="AK15">
         <f t="shared" si="8"/>
-        <v>0.15217391304347827</v>
+        <v>7.6045627376425853E-2</v>
       </c>
       <c r="AL15">
         <f t="shared" si="9"/>
-        <v>0.19565217391304349</v>
+        <v>9.8859315589353611E-2</v>
       </c>
       <c r="AM15">
         <f t="shared" si="10"/>
-        <v>6.5217391304347824E-2</v>
+        <v>9.1254752851711016E-2</v>
       </c>
       <c r="AN15">
         <f t="shared" si="11"/>
@@ -10446,19 +10445,19 @@
       </c>
       <c r="AO15">
         <f t="shared" si="12"/>
-        <v>2.1739130434782612E-2</v>
+        <v>3.8022813688212927E-2</v>
       </c>
       <c r="AP15">
         <f t="shared" ref="AP15:AP18" si="15">Y15/F15</f>
-        <v>6.5217391304347824E-2</v>
+        <v>1.9011406844106463E-2</v>
       </c>
       <c r="AQ15">
         <f t="shared" si="13"/>
-        <v>6.5217391304347824E-2</v>
+        <v>9.8859315589353611E-2</v>
       </c>
       <c r="AR15">
         <f t="shared" si="14"/>
-        <v>0.41304347826086957</v>
+        <v>0.32699619771863114</v>
       </c>
     </row>
     <row r="16" spans="2:44" x14ac:dyDescent="0.2">
@@ -10611,7 +10610,7 @@
       </c>
       <c r="AN16">
         <f t="shared" si="11"/>
-        <v>6.5217391304347824E-2</v>
+        <v>0.10059171597633136</v>
       </c>
       <c r="AO16">
         <f t="shared" si="12"/>
@@ -10632,184 +10631,184 @@
     </row>
     <row r="17" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B17" s="191" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C17" s="192" t="str">
         <f>VLOOKUP($B17,$B$63:$AA$76,C$11,FALSE)</f>
-        <v>F</v>
+        <v>G</v>
       </c>
       <c r="D17" s="192" t="str">
         <f>VLOOKUP($B17,$B$63:$AA$76,D$11,FALSE)</f>
-        <v>6'3"</v>
+        <v>6'0"</v>
       </c>
       <c r="E17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,E$11,FALSE)</f>
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,F$11,FALSE)</f>
-        <v>4.5999999999999996</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="G17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,G$11,FALSE)</f>
-        <v>0.6</v>
+        <v>2.1</v>
       </c>
       <c r="H17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,H$11,FALSE)</f>
-        <v>1.4</v>
+        <v>4.7</v>
       </c>
       <c r="I17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,I$11,FALSE)</f>
-        <v>44</v>
+        <v>44.2</v>
       </c>
       <c r="J17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,J$11,FALSE)</f>
-        <v>0.6</v>
+        <v>1.7</v>
       </c>
       <c r="K17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,K$11,FALSE)</f>
-        <v>1.4</v>
+        <v>3.5</v>
       </c>
       <c r="L17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,L$11,FALSE)</f>
-        <v>44</v>
+        <v>48.1</v>
       </c>
       <c r="M17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,M$11,FALSE)</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="N17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,N$11,FALSE)</f>
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="O17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,O$11,FALSE)</f>
-        <v>0</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="P17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,P$11,FALSE)</f>
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,Q$11,FALSE)</f>
-        <v>0.9</v>
+        <v>1.4</v>
       </c>
       <c r="R17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,R$11,FALSE)</f>
-        <v>70.599999999999994</v>
+        <v>72.099999999999994</v>
       </c>
       <c r="S17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,S$11,FALSE)</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="T17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,T$11,FALSE)</f>
-        <v>0.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="U17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,U$11,FALSE)</f>
-        <v>1.6</v>
+        <v>3.3</v>
       </c>
       <c r="V17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,V$11,FALSE)</f>
-        <v>0.3</v>
+        <v>1.7</v>
       </c>
       <c r="W17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,W$11,FALSE)</f>
-        <v>0.3</v>
+        <v>1.7</v>
       </c>
       <c r="X17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,X$11,FALSE)</f>
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="Y17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,Y$11,FALSE)</f>
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="Z17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,Z$11,FALSE)</f>
-        <v>0.3</v>
+        <v>1.3</v>
       </c>
       <c r="AA17" s="192">
         <f>VLOOKUP($B17,$B$63:$AA$76,AA$11,FALSE)</f>
-        <v>1.9</v>
+        <v>5.6</v>
       </c>
       <c r="AC17">
         <f t="shared" si="0"/>
-        <v>0.19565217391304349</v>
+        <v>5.9171597633136098E-2</v>
       </c>
       <c r="AD17">
         <f t="shared" si="1"/>
-        <v>0.15217391304347827</v>
+        <v>0.13609467455621302</v>
       </c>
       <c r="AE17">
         <f t="shared" si="2"/>
-        <v>0.13043478260869565</v>
+        <v>0.12426035502958581</v>
       </c>
       <c r="AF17">
         <f t="shared" si="3"/>
-        <v>0.30434782608695654</v>
+        <v>0.27810650887573968</v>
       </c>
       <c r="AG17">
         <f t="shared" si="4"/>
-        <v>0.13043478260869565</v>
+        <v>0.10059171597633136</v>
       </c>
       <c r="AH17">
         <f t="shared" si="5"/>
-        <v>0.30434782608695654</v>
+        <v>0.20710059171597636</v>
       </c>
       <c r="AI17">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.3668639053254441E-2</v>
       </c>
       <c r="AJ17">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="AK17">
         <f t="shared" si="8"/>
-        <v>0.15217391304347827</v>
+        <v>5.9171597633136098E-2</v>
       </c>
       <c r="AL17">
         <f t="shared" si="9"/>
-        <v>0.19565217391304349</v>
+        <v>8.2840236686390539E-2</v>
       </c>
       <c r="AM17">
         <f t="shared" si="10"/>
-        <v>6.5217391304347824E-2</v>
+        <v>0.10059171597633136</v>
       </c>
       <c r="AN17">
         <f t="shared" si="11"/>
-        <v>8.3650190114068448E-2</v>
+        <v>8.2352941176470587E-2</v>
       </c>
       <c r="AO17">
         <f t="shared" si="12"/>
-        <v>2.1739130434782612E-2</v>
+        <v>5.3254437869822494E-2</v>
       </c>
       <c r="AP17">
         <f t="shared" si="15"/>
-        <v>6.5217391304347824E-2</v>
+        <v>5.9171597633136102E-3</v>
       </c>
       <c r="AQ17">
         <f t="shared" si="13"/>
-        <v>6.5217391304347824E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="AR17">
         <f t="shared" si="14"/>
-        <v>0.41304347826086957</v>
+        <v>0.33136094674556216</v>
       </c>
     </row>
     <row r="18" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B18" s="193" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C18" s="192" t="str">
         <f>VLOOKUP($B18,$B$63:$AA$76,C$11,FALSE)</f>
-        <v>G</v>
+        <v>C</v>
       </c>
       <c r="D18" s="192" t="str">
         <f>VLOOKUP($B18,$B$63:$AA$76,D$11,FALSE)</f>
-        <v>5'10"</v>
+        <v>6'5"</v>
       </c>
       <c r="E18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,E$11,FALSE)</f>
@@ -10817,135 +10816,135 @@
       </c>
       <c r="F18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,F$11,FALSE)</f>
-        <v>26.3</v>
+        <v>25.5</v>
       </c>
       <c r="G18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,G$11,FALSE)</f>
-        <v>3</v>
+        <v>4.7</v>
       </c>
       <c r="H18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,H$11,FALSE)</f>
-        <v>7.9</v>
+        <v>8.9</v>
       </c>
       <c r="I18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,I$11,FALSE)</f>
-        <v>38.1</v>
+        <v>52.8</v>
       </c>
       <c r="J18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,J$11,FALSE)</f>
-        <v>2.4</v>
+        <v>4.7</v>
       </c>
       <c r="K18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,K$11,FALSE)</f>
-        <v>5.9</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="L18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,L$11,FALSE)</f>
-        <v>40</v>
+        <v>53.9</v>
       </c>
       <c r="M18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,M$11,FALSE)</f>
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="N18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,N$11,FALSE)</f>
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="O18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,O$11,FALSE)</f>
-        <v>32.4</v>
+        <v>0</v>
       </c>
       <c r="P18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,P$11,FALSE)</f>
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="Q18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,Q$11,FALSE)</f>
-        <v>2.6</v>
+        <v>3.3</v>
       </c>
       <c r="R18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,R$11,FALSE)</f>
-        <v>75.3</v>
+        <v>73.2</v>
       </c>
       <c r="S18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,S$11,FALSE)</f>
-        <v>0.7</v>
+        <v>1.8</v>
       </c>
       <c r="T18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,T$11,FALSE)</f>
-        <v>3.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="U18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,U$11,FALSE)</f>
-        <v>3.9</v>
+        <v>5.9</v>
       </c>
       <c r="V18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,V$11,FALSE)</f>
-        <v>2.4</v>
+        <v>1.8</v>
       </c>
       <c r="W18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,W$11,FALSE)</f>
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="X18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,X$11,FALSE)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,Y$11,FALSE)</f>
-        <v>0.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Z18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,Z$11,FALSE)</f>
-        <v>2.6</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AA18" s="192">
         <f>VLOOKUP($B18,$B$63:$AA$76,AA$11,FALSE)</f>
-        <v>8.6</v>
+        <v>11.8</v>
       </c>
       <c r="AC18">
         <f t="shared" si="0"/>
-        <v>2.6615969581749048E-2</v>
+        <v>7.0588235294117646E-2</v>
       </c>
       <c r="AD18">
         <f t="shared" si="1"/>
-        <v>0.12167300380228137</v>
+        <v>0.16078431372549018</v>
       </c>
       <c r="AE18">
         <f t="shared" si="2"/>
-        <v>0.11406844106463879</v>
+        <v>0.18431372549019609</v>
       </c>
       <c r="AF18">
         <f t="shared" si="3"/>
-        <v>0.30038022813688214</v>
+        <v>0.34901960784313729</v>
       </c>
       <c r="AG18">
         <f t="shared" si="4"/>
-        <v>9.1254752851711016E-2</v>
+        <v>0.18431372549019609</v>
       </c>
       <c r="AH18">
         <f t="shared" si="5"/>
-        <v>0.22433460076045628</v>
+        <v>0.34117647058823525</v>
       </c>
       <c r="AI18">
         <f t="shared" si="6"/>
-        <v>2.2813688212927754E-2</v>
+        <v>0</v>
       </c>
       <c r="AJ18">
         <f t="shared" si="7"/>
-        <v>7.6045627376425853E-2</v>
+        <v>7.8431372549019607E-3</v>
       </c>
       <c r="AK18">
         <f t="shared" si="8"/>
-        <v>7.6045627376425853E-2</v>
+        <v>9.4117647058823528E-2</v>
       </c>
       <c r="AL18">
         <f t="shared" si="9"/>
-        <v>9.8859315589353611E-2</v>
+        <v>0.12941176470588234</v>
       </c>
       <c r="AM18">
         <f t="shared" si="10"/>
-        <v>9.1254752851711016E-2</v>
+        <v>7.0588235294117646E-2</v>
       </c>
       <c r="AN18" t="e">
         <f>#REF!/#REF!</f>
@@ -10953,19 +10952,19 @@
       </c>
       <c r="AO18">
         <f t="shared" si="12"/>
-        <v>3.8022813688212927E-2</v>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="AP18">
         <f t="shared" si="15"/>
-        <v>1.9011406844106463E-2</v>
+        <v>4.3137254901960791E-2</v>
       </c>
       <c r="AQ18">
         <f t="shared" si="13"/>
-        <v>9.8859315589353611E-2</v>
+        <v>9.0196078431372548E-2</v>
       </c>
       <c r="AR18">
         <f t="shared" si="14"/>
-        <v>0.32699619771863114</v>
+        <v>0.46274509803921571</v>
       </c>
     </row>
     <row r="19" spans="2:44" x14ac:dyDescent="0.2">
@@ -10978,87 +10977,87 @@
       <c r="F19" s="192"/>
       <c r="G19" s="192">
         <f t="shared" ref="G19:V19" si="16">((G14/$F14)+(G15/$F15)+(G16/$F16)+(G17/$F17)+(G18/$F18))*40</f>
-        <v>24.061065401782873</v>
+        <v>31.555406578205002</v>
       </c>
       <c r="H19" s="192">
         <f t="shared" si="16"/>
-        <v>63.500158958251205</v>
+        <v>64.643826985800516</v>
       </c>
       <c r="I19" s="195">
         <f>G19/H19</f>
-        <v>0.37891346724977576</v>
+        <v>0.48814261236631884</v>
       </c>
       <c r="J19" s="192">
         <f t="shared" si="16"/>
-        <v>18.927782087312586</v>
+        <v>27.783070009296843</v>
       </c>
       <c r="K19" s="192">
         <f t="shared" si="16"/>
-        <v>45.067029515368084</v>
+        <v>53.056735366330784</v>
       </c>
       <c r="L19" s="195">
         <f>J19/K19</f>
-        <v>0.41999178314732544</v>
+        <v>0.52364831378086774</v>
       </c>
       <c r="M19" s="192">
         <f t="shared" si="16"/>
-        <v>4.3640525452395185</v>
+        <v>3.772336568908158</v>
       </c>
       <c r="N19" s="192">
         <f t="shared" si="16"/>
-        <v>18.433129442883121</v>
+        <v>11.823778010002277</v>
       </c>
       <c r="O19" s="195">
         <f>M19/N19</f>
-        <v>0.23675049636915793</v>
+        <v>0.31904663346326068</v>
       </c>
       <c r="P19" s="192">
         <f t="shared" si="16"/>
-        <v>17.37627325559215</v>
+        <v>14.582166479469802</v>
       </c>
       <c r="Q19" s="192">
         <f t="shared" si="16"/>
-        <v>23.058051553340029</v>
+        <v>20.820378253595798</v>
       </c>
       <c r="R19" s="195">
         <f>P19/Q19</f>
-        <v>0.7535880998182235</v>
+        <v>0.70037951769446738</v>
       </c>
       <c r="S19" s="192">
         <f t="shared" si="16"/>
-        <v>20.415809351831836</v>
+        <v>13.934546055173097</v>
       </c>
       <c r="T19" s="192">
         <f t="shared" si="16"/>
-        <v>23.970599081857141</v>
+        <v>28.07224866000643</v>
       </c>
       <c r="U19" s="192">
         <f t="shared" si="16"/>
-        <v>45.329552246398009</v>
+        <v>42.180707758657789</v>
       </c>
       <c r="V19" s="192">
         <f t="shared" si="16"/>
-        <v>13.857547973600216</v>
+        <v>14.331829023059935</v>
       </c>
       <c r="W19" s="192">
         <f>((W14/$F14)+(W15/$F15)+(W16/$F16)+(W17/$F17)+(W18/$F18))*40</f>
-        <v>12.536643056067753</v>
+        <v>16.592026281029856</v>
       </c>
       <c r="X19" s="192">
         <f>((X14/$F14)+(X15/$F15)+(X16/$F16)+(X17/$F17)+(X18/$F18))*40</f>
-        <v>5.4205780993679822</v>
+        <v>7.5734330264673932</v>
       </c>
       <c r="Y19" s="192">
         <f>((Y14/$F14)+(Y15/$F15)+(Y16/$F16)+(Y17/$F17)+(Y18/$F18))*40</f>
-        <v>7.6166435647341579</v>
+        <v>3.9415430559324784</v>
       </c>
       <c r="Z19" s="192">
         <f t="shared" ref="Z19" si="17">SUM(AQ14:AQ18)*40</f>
-        <v>13.145008075079161</v>
+        <v>17.266061184439042</v>
       </c>
       <c r="AA19" s="192">
         <f>2*J19 +3*M19 + P19</f>
-        <v>68.323995065935875</v>
+        <v>81.465316204787968</v>
       </c>
     </row>
     <row r="20" spans="2:44" x14ac:dyDescent="0.2">
@@ -11280,7 +11279,7 @@
     </row>
     <row r="25" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B25" s="198" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C25" s="192" t="str">
         <f>VLOOKUP($B25,$B$47:$T$60,C$11,FALSE)</f>
@@ -11288,76 +11287,76 @@
       </c>
       <c r="D25" s="192" t="str">
         <f>VLOOKUP($B25,$B$47:$T$60,D$11,FALSE)</f>
-        <v>5'10"</v>
+        <v>6'0"</v>
       </c>
       <c r="E25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,E$11,FALSE)</f>
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,F$11,FALSE)</f>
-        <v>26.3</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="G25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,G$11,FALSE)</f>
-        <v>20.399999999999999</v>
+        <v>19.8</v>
       </c>
       <c r="H25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,H$11,FALSE)</f>
-        <v>0.94</v>
+        <v>1.04</v>
       </c>
       <c r="I25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,I$11,FALSE)</f>
-        <v>42.2</v>
+        <v>48.6</v>
       </c>
       <c r="J25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,J$11,FALSE)</f>
-        <v>21.9</v>
+        <v>23.3</v>
       </c>
       <c r="K25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,K$11,FALSE)</f>
-        <v>17.399999999999999</v>
+        <v>15.9</v>
       </c>
       <c r="L25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,L$11,FALSE)</f>
-        <v>3.1</v>
+        <v>6.5</v>
       </c>
       <c r="M25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,M$11,FALSE)</f>
-        <v>13.5</v>
+        <v>14.9</v>
       </c>
       <c r="N25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,N$11,FALSE)</f>
-        <v>8.3000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="O25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,O$11,FALSE)</f>
-        <v>16.7</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="P25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,P$11,FALSE)</f>
-        <v>19.5</v>
+        <v>24</v>
       </c>
       <c r="Q25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,Q$11,FALSE)</f>
-        <v>1.1100000000000001</v>
+        <v>0.98</v>
       </c>
       <c r="R25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,R$11,FALSE)</f>
-        <v>2.1</v>
+        <v>2.9</v>
       </c>
       <c r="S25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,S$11,FALSE)</f>
-        <v>2</v>
+        <v>0.8</v>
       </c>
       <c r="T25" s="192">
         <f>VLOOKUP($B25,$B$47:$T$60,T$11,FALSE)</f>
-        <v>5.7</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="26" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B26" s="198" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C26" s="192" t="str">
         <f>VLOOKUP($B26,$B$47:$T$60,C$11,FALSE)</f>
@@ -11365,71 +11364,71 @@
       </c>
       <c r="D26" s="192" t="str">
         <f>VLOOKUP($B26,$B$47:$T$60,D$11,FALSE)</f>
-        <v>5'11"</v>
+        <v>6'0"</v>
       </c>
       <c r="E26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,E$11,FALSE)</f>
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="F26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,F$11,FALSE)</f>
-        <v>31</v>
+        <v>5.2</v>
       </c>
       <c r="G26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,G$11,FALSE)</f>
-        <v>16</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="H26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,H$11,FALSE)</f>
-        <v>1.1399999999999999</v>
+        <v>0.64</v>
       </c>
       <c r="I26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,I$11,FALSE)</f>
-        <v>52.6</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="J26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,J$11,FALSE)</f>
-        <v>59.2</v>
+        <v>63.8</v>
       </c>
       <c r="K26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,K$11,FALSE)</f>
-        <v>25.5</v>
+        <v>16</v>
       </c>
       <c r="L26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,L$11,FALSE)</f>
-        <v>1</v>
+        <v>6.8</v>
       </c>
       <c r="M26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,M$11,FALSE)</f>
-        <v>9.8000000000000007</v>
+        <v>5.3</v>
       </c>
       <c r="N26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,N$11,FALSE)</f>
-        <v>5.5</v>
+        <v>6.1</v>
       </c>
       <c r="O26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,O$11,FALSE)</f>
-        <v>6.7</v>
+        <v>14.7</v>
       </c>
       <c r="P26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,P$11,FALSE)</f>
-        <v>14.3</v>
+        <v>8.4</v>
       </c>
       <c r="Q26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,Q$11,FALSE)</f>
-        <v>0.78</v>
+        <v>2.33</v>
       </c>
       <c r="R26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,R$11,FALSE)</f>
-        <v>1.9</v>
+        <v>1.4</v>
       </c>
       <c r="S26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,S$11,FALSE)</f>
-        <v>0.4</v>
+        <v>1.3</v>
       </c>
       <c r="T26" s="192">
         <f>VLOOKUP($B26,$B$47:$T$60,T$11,FALSE)</f>
-        <v>4.2</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="27" spans="2:44" x14ac:dyDescent="0.2">
@@ -11511,7 +11510,7 @@
     </row>
     <row r="28" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B28" s="199" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C28" s="192" t="str">
         <f>VLOOKUP($B28,$B$47:$T$60,C$11,FALSE)</f>
@@ -11519,71 +11518,71 @@
       </c>
       <c r="D28" s="192" t="str">
         <f>VLOOKUP($B28,$B$47:$T$60,D$11,FALSE)</f>
-        <v>5'8"</v>
+        <v>5'10"</v>
       </c>
       <c r="E28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,E$11,FALSE)</f>
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,F$11,FALSE)</f>
-        <v>4.4000000000000004</v>
+        <v>26.3</v>
       </c>
       <c r="G28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,G$11,FALSE)</f>
-        <v>11.3</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="H28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,H$11,FALSE)</f>
-        <v>0.65</v>
+        <v>0.94</v>
       </c>
       <c r="I28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,I$11,FALSE)</f>
-        <v>26.9</v>
+        <v>42.2</v>
       </c>
       <c r="J28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,J$11,FALSE)</f>
-        <v>43</v>
+        <v>21.9</v>
       </c>
       <c r="K28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,K$11,FALSE)</f>
-        <v>11.9</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="L28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,L$11,FALSE)</f>
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="M28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,M$11,FALSE)</f>
-        <v>4.5999999999999996</v>
+        <v>13.5</v>
       </c>
       <c r="N28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,N$11,FALSE)</f>
-        <v>4.0999999999999996</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="O28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,O$11,FALSE)</f>
-        <v>22.8</v>
+        <v>16.7</v>
       </c>
       <c r="P28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,P$11,FALSE)</f>
-        <v>39.200000000000003</v>
+        <v>19.5</v>
       </c>
       <c r="Q28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,Q$11,FALSE)</f>
-        <v>1.56</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="R28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,R$11,FALSE)</f>
-        <v>5.3</v>
+        <v>2.1</v>
       </c>
       <c r="S28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,S$11,FALSE)</f>
-        <v>1.1000000000000001</v>
+        <v>2</v>
       </c>
       <c r="T28" s="192">
         <f>VLOOKUP($B28,$B$47:$T$60,T$11,FALSE)</f>
-        <v>3.5</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="29" spans="2:44" x14ac:dyDescent="0.2">
@@ -11595,63 +11594,63 @@
       <c r="E29" s="197"/>
       <c r="F29" s="197">
         <f t="shared" ref="F29:T29" si="18">AVERAGE(F$24:F$28)</f>
-        <v>23.14</v>
+        <v>20.479999999999997</v>
       </c>
       <c r="G29" s="197">
         <f t="shared" si="18"/>
-        <v>16.52</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="H29" s="197">
         <f t="shared" si="18"/>
-        <v>0.97399999999999998</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="I29" s="197">
         <f t="shared" si="18"/>
-        <v>44.58</v>
+        <v>44.86</v>
       </c>
       <c r="J29" s="197">
         <f t="shared" si="18"/>
-        <v>44.6</v>
+        <v>41.58</v>
       </c>
       <c r="K29" s="197">
         <f t="shared" si="18"/>
-        <v>18.380000000000003</v>
+        <v>17.28</v>
       </c>
       <c r="L29" s="197">
         <f t="shared" si="18"/>
-        <v>2.54</v>
+        <v>4.3</v>
       </c>
       <c r="M29" s="197">
         <f t="shared" si="18"/>
-        <v>10.56</v>
+        <v>11.72</v>
       </c>
       <c r="N29" s="197">
         <f t="shared" si="18"/>
-        <v>6.62</v>
+        <v>8.0799999999999983</v>
       </c>
       <c r="O29" s="197">
         <f t="shared" si="18"/>
-        <v>12.279999999999998</v>
+        <v>12.940000000000001</v>
       </c>
       <c r="P29" s="197">
         <f t="shared" si="18"/>
-        <v>20.54</v>
+        <v>16.32</v>
       </c>
       <c r="Q29" s="197">
         <f t="shared" si="18"/>
-        <v>0.99600000000000011</v>
+        <v>1.19</v>
       </c>
       <c r="R29" s="197">
         <f t="shared" si="18"/>
-        <v>2.62</v>
+        <v>2.04</v>
       </c>
       <c r="S29" s="197">
         <f t="shared" si="18"/>
-        <v>1.2599999999999998</v>
+        <v>1.3800000000000001</v>
       </c>
       <c r="T29" s="197">
         <f t="shared" si="18"/>
-        <v>4.2200000000000006</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="30" spans="2:44" x14ac:dyDescent="0.2">
@@ -13765,6 +13764,210 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G19:G20">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19:H20">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19:I20">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19:J20">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19:K20">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:L20">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M19:M20">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W19:W20">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z19:Z20">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R19:R20">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q19:Q20">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P19:P20">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O19:O20">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N19:N20">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S19:S20">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T19:T20">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U19:U20">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V19:V20">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -13776,7 +13979,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H19:H20">
+  <conditionalFormatting sqref="X19:X20">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -13788,7 +13991,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I19:I20">
+  <conditionalFormatting sqref="Y19:Y20">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -13800,7 +14003,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J19:J20">
+  <conditionalFormatting sqref="AA19:AA20">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -13812,7 +14015,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K19:K20">
+  <conditionalFormatting sqref="G24:G28">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -13824,7 +14027,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19:L20">
+  <conditionalFormatting sqref="H24:H28">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -13836,7 +14039,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M19:M20">
+  <conditionalFormatting sqref="I24:I28">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -13848,7 +14051,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W19:W20">
+  <conditionalFormatting sqref="P24:P28">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -13860,7 +14063,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z19:Z20">
+  <conditionalFormatting sqref="T24:T28">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -13872,7 +14075,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R19:R20">
+  <conditionalFormatting sqref="J24:J29">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -13884,7 +14087,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q19:Q20">
+  <conditionalFormatting sqref="K24:K28">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -13896,7 +14099,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P19:P20">
+  <conditionalFormatting sqref="L24:L28">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -13908,7 +14111,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O19:O20">
+  <conditionalFormatting sqref="M24:M28">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -13920,7 +14123,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N19:N20">
+  <conditionalFormatting sqref="N24:N28">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -13932,7 +14135,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S19:S20">
+  <conditionalFormatting sqref="O24:O28">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -13944,7 +14147,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T19:T20">
+  <conditionalFormatting sqref="Q24:Q28">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -13956,7 +14159,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U19:U20">
+  <conditionalFormatting sqref="R24:R28">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -13968,7 +14171,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V19:V20">
+  <conditionalFormatting sqref="S24:S28">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -13980,7 +14183,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X19:X20">
+  <conditionalFormatting sqref="F24:F28">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -13992,7 +14195,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y19:Y20">
+  <conditionalFormatting sqref="E24:E28">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -14004,7 +14207,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA19:AA20">
+  <conditionalFormatting sqref="D24:D28">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -14024,18 +14227,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFE229E-C643-2B4F-B7AA-2D418CBAB565}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>